<commit_message>
testing recent updates to see if they push to heroku
</commit_message>
<xml_diff>
--- a/support_docs/Final Project Matrix.xlsx
+++ b/support_docs/Final Project Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Brown\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bd11a8894b05b05/Desktop/Homework/Team5_FinalProject/support_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484529C0-8D5C-490D-8A27-A5062EFA29CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{484529C0-8D5C-490D-8A27-A5062EFA29CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{290CA192-4845-4E81-AEB4-A26DDEDB9454}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC9A98B1-368D-4B37-B1B8-9F5BE48DC783}"/>
+    <workbookView xWindow="46275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{AC9A98B1-368D-4B37-B1B8-9F5BE48DC783}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +188,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -676,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -692,12 +698,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -710,137 +710,146 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1159,7 +1168,7 @@
   <dimension ref="B3:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="R8" sqref="R8:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1171,7 +1180,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="39" t="s">
         <v>33</v>
       </c>
       <c r="D3" t="s">
@@ -1180,45 +1189,45 @@
     </row>
     <row r="5" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="2:22" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="21"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="47"/>
+      <c r="C6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="45"/>
+      <c r="E6" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="16" t="s">
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="37"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="6" t="s">
+      <c r="K6" s="41"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="28"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="7"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="50"/>
+      <c r="V6" s="45"/>
     </row>
     <row r="7" spans="2:22" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="22"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -1230,10 +1239,10 @@
       <c r="H7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -1251,55 +1260,55 @@
       <c r="O7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="Q7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="S7" s="19" t="s">
+      <c r="S7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="T7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="U7" s="27" t="s">
+      <c r="U7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="20" t="s">
+      <c r="V7" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:22" ht="25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="20" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="30" t="s">
+      <c r="I8" s="21"/>
+      <c r="J8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="K8" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="36" t="s">
+      <c r="L8" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="43" t="s">
+      <c r="M8" s="28" t="s">
         <v>32</v>
       </c>
       <c r="N8" s="3" t="s">
@@ -1308,35 +1317,35 @@
       <c r="O8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="50" t="s">
+      <c r="P8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="30" t="s">
+      <c r="Q8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="R8" s="51" t="s">
+      <c r="R8" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="S8" s="36" t="s">
+      <c r="S8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="T8" s="36" t="s">
+      <c r="T8" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="U8" s="54" t="s">
+      <c r="U8" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="V8" s="10"/>
+      <c r="V8" s="8"/>
     </row>
     <row r="9" spans="2:22" ht="50.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="33"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
         <v>25</v>
@@ -1344,32 +1353,32 @@
       <c r="H9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="33" t="s">
+      <c r="I9" s="19"/>
+      <c r="J9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="44" t="s">
+      <c r="M9" s="29" t="s">
         <v>32</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="47" t="s">
+      <c r="O9" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="P9" s="31" t="s">
+      <c r="P9" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="33" t="s">
+      <c r="Q9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="R9" s="52" t="s">
+      <c r="R9" s="58" t="s">
         <v>27</v>
       </c>
       <c r="S9" s="2" t="s">
@@ -1378,53 +1387,53 @@
       <c r="T9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U9" s="55" t="s">
+      <c r="U9" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="V9" s="29" t="s">
+      <c r="V9" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:22" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="29" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="33"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="38" t="s">
+      <c r="I10" s="19"/>
+      <c r="J10" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="57" t="s">
+      <c r="K10" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="40" t="s">
+      <c r="L10" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="M10" s="43" t="s">
+      <c r="M10" s="28" t="s">
         <v>32</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="47" t="s">
+      <c r="O10" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="50" t="s">
+      <c r="P10" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="Q10" s="38" t="s">
+      <c r="Q10" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="R10" s="52" t="s">
+      <c r="R10" s="58" t="s">
         <v>27</v>
       </c>
       <c r="S10" s="2" t="s">
@@ -1433,63 +1442,63 @@
       <c r="T10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U10" s="55" t="s">
+      <c r="U10" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="V10" s="12"/>
+      <c r="V10" s="10"/>
     </row>
     <row r="11" spans="2:22" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="32" t="s">
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="42" t="s">
+      <c r="K11" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="35" t="s">
+      <c r="L11" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="45" t="s">
+      <c r="M11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="46" t="s">
+      <c r="N11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="O11" s="48" t="s">
+      <c r="O11" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="49" t="s">
+      <c r="P11" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="34" t="s">
+      <c r="Q11" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="R11" s="53" t="s">
+      <c r="R11" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="S11" s="35" t="s">
+      <c r="S11" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="T11" s="35" t="s">
+      <c r="T11" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="U11" s="56" t="s">
+      <c r="U11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="V11" s="14"/>
+      <c r="V11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>